<commit_message>
Musical Score Encoding Test & Simple Integer DNA Encoding
</commit_message>
<xml_diff>
--- a/DDDS System/DataSet/Testing_Data_Set/Result.xlsx
+++ b/DDDS System/DataSet/Testing_Data_Set/Result.xlsx
@@ -696,86 +696,86 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1059,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1076,18 +1076,18 @@
   <sheetData>
     <row r="1" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
       <c r="M2" s="19" t="s">
         <v>1</v>
       </c>
@@ -1111,30 +1111,30 @@
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="43"/>
-      <c r="M3" s="25">
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
+      <c r="M3" s="49">
         <v>1.5</v>
       </c>
-      <c r="N3" s="23">
+      <c r="N3" s="48">
         <v>1</v>
       </c>
       <c r="O3" s="16">
         <v>0.5</v>
       </c>
       <c r="P3" s="13">
-        <v>8.7239599999999999</v>
+        <v>5.6175600000000001</v>
       </c>
       <c r="Q3" s="5">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="R3" s="5">
         <v>0</v>
@@ -1144,26 +1144,26 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="46"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="24"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="40"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="45"/>
       <c r="O4" s="17">
         <v>1</v>
       </c>
       <c r="P4" s="14">
-        <v>13.076599999999999</v>
+        <v>9.0215800000000002</v>
       </c>
       <c r="Q4" s="1">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="R4" s="1">
         <v>0</v>
@@ -1183,16 +1183,16 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="9"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="24"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="45"/>
       <c r="O5" s="17">
         <v>2</v>
       </c>
       <c r="P5" s="14">
-        <v>22.823699999999999</v>
+        <v>15.271599999999999</v>
       </c>
       <c r="Q5" s="1">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="R5" s="1">
         <v>0</v>
@@ -1202,28 +1202,28 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="33"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="24"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="27"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="45"/>
       <c r="O6" s="17">
         <v>4</v>
       </c>
       <c r="P6" s="14">
-        <v>34.170400000000001</v>
+        <v>28.720199999999998</v>
       </c>
       <c r="Q6" s="1">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="R6" s="1">
         <v>0</v>
@@ -1233,26 +1233,26 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="34"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="24"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="17">
         <v>8</v>
       </c>
       <c r="P7" s="14">
-        <v>51.915900000000001</v>
+        <v>48.363100000000003</v>
       </c>
       <c r="Q7" s="1">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="R7" s="1">
         <v>0</v>
@@ -1262,28 +1262,28 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="34"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="24">
+      <c r="B8" s="28"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="45">
         <v>4</v>
       </c>
       <c r="O8" s="17">
         <v>0.5</v>
       </c>
       <c r="P8" s="14">
-        <v>1.2090799999999999</v>
+        <v>0.68824399999999997</v>
       </c>
       <c r="Q8" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="R8" s="1">
         <v>0</v>
@@ -1293,26 +1293,26 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="34"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="24"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="45"/>
       <c r="O9" s="17">
         <v>1</v>
       </c>
       <c r="P9" s="14">
-        <v>2.1763400000000002</v>
+        <v>0.98586300000000004</v>
       </c>
       <c r="Q9" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="R9" s="1">
         <v>0</v>
@@ -1332,16 +1332,16 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="24"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="45"/>
       <c r="O10" s="17">
         <v>2</v>
       </c>
       <c r="P10" s="14">
-        <v>7.7381000000000002</v>
+        <v>2.2321399999999998</v>
       </c>
       <c r="Q10" s="1">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="R10" s="1">
         <v>0</v>
@@ -1351,28 +1351,28 @@
       </c>
     </row>
     <row r="11" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="48"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="24"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="42"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="45"/>
       <c r="O11" s="17">
         <v>4</v>
       </c>
       <c r="P11" s="14">
-        <v>15.6622</v>
+        <v>3.1808000000000001</v>
       </c>
       <c r="Q11" s="1">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="R11" s="1">
         <v>0</v>
@@ -1382,26 +1382,26 @@
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="49"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="48"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="24"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="42"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="45"/>
       <c r="O12" s="17">
         <v>8</v>
       </c>
       <c r="P12" s="14">
-        <v>32.012599999999999</v>
+        <v>17.9315</v>
       </c>
       <c r="Q12" s="1">
-        <v>150</v>
+        <v>32</v>
       </c>
       <c r="R12" s="1">
         <v>0</v>
@@ -1411,28 +1411,28 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="49"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="48"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="24">
+      <c r="B13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="42"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="45">
         <v>16</v>
       </c>
       <c r="O13" s="17">
         <v>0.5</v>
       </c>
       <c r="P13" s="14">
-        <v>1.0974699999999999</v>
+        <v>0.68824399999999997</v>
       </c>
       <c r="Q13" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R13" s="1">
         <v>0</v>
@@ -1442,26 +1442,26 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B14" s="49"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="48"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="24"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="42"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="45"/>
       <c r="O14" s="17">
         <v>1</v>
       </c>
       <c r="P14" s="14">
-        <v>1.1160699999999999</v>
+        <v>0.68824399999999997</v>
       </c>
       <c r="Q14" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R14" s="1">
         <v>0</v>
@@ -1471,26 +1471,26 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B15" s="49"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="48"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="24"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="42"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="45"/>
       <c r="O15" s="17">
         <v>2</v>
       </c>
       <c r="P15" s="14">
-        <v>1.2462800000000001</v>
+        <v>1.93452</v>
       </c>
       <c r="Q15" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="R15" s="1">
         <v>0</v>
@@ -1500,26 +1500,26 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B16" s="49"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="48"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="24"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="42"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="45"/>
       <c r="O16" s="17">
         <v>4</v>
       </c>
       <c r="P16" s="14">
-        <v>1.3020799999999999</v>
+        <v>2.6599699999999999</v>
       </c>
       <c r="Q16" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="R16" s="1">
         <v>0</v>
@@ -1529,26 +1529,26 @@
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B17" s="49"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="48"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="24"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="42"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="45"/>
       <c r="O17" s="17">
         <v>8</v>
       </c>
       <c r="P17" s="14">
-        <v>1.46949</v>
+        <v>4.1294599999999999</v>
       </c>
       <c r="Q17" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="R17" s="1">
         <v>0</v>
@@ -1558,30 +1558,30 @@
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B18" s="49"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="48"/>
-      <c r="M18" s="26">
+      <c r="B18" s="43"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="42"/>
+      <c r="M18" s="44">
         <v>2</v>
       </c>
-      <c r="N18" s="24">
+      <c r="N18" s="45">
         <v>1</v>
       </c>
       <c r="O18" s="17">
         <v>0.5</v>
       </c>
       <c r="P18" s="14">
-        <v>6.8452400000000004</v>
+        <v>3.49702</v>
       </c>
       <c r="Q18" s="1">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="R18" s="1">
         <v>0</v>
@@ -1591,26 +1591,26 @@
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B19" s="49"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="48"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="24"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="42"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="17">
         <v>1</v>
       </c>
       <c r="P19" s="14">
-        <v>10.4725</v>
+        <v>6.3057999999999996</v>
       </c>
       <c r="Q19" s="1">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
@@ -1620,26 +1620,26 @@
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B20" s="49"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="48"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="24"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="42"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="45"/>
       <c r="O20" s="17">
         <v>2</v>
       </c>
       <c r="P20" s="14">
-        <v>16.871300000000002</v>
+        <v>12.128</v>
       </c>
       <c r="Q20" s="1">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="R20" s="1">
         <v>0</v>
@@ -1649,26 +1649,26 @@
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="49"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="48"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="24"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="42"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="45"/>
       <c r="O21" s="17">
         <v>4</v>
       </c>
       <c r="P21" s="14">
-        <v>31.789400000000001</v>
+        <v>22.6004</v>
       </c>
       <c r="Q21" s="1">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="R21" s="1">
         <v>0</v>
@@ -1678,26 +1678,26 @@
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="49"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="48"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="24"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="42"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="45"/>
       <c r="O22" s="17">
         <v>8</v>
       </c>
       <c r="P22" s="14">
-        <v>41.257399999999997</v>
+        <v>36.886200000000002</v>
       </c>
       <c r="Q22" s="1">
-        <v>130</v>
+        <v>74</v>
       </c>
       <c r="R22" s="1">
         <v>0</v>
@@ -1707,28 +1707,28 @@
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B23" s="49"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="48"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="24">
+      <c r="B23" s="43"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="42"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="45">
         <v>4</v>
       </c>
       <c r="O23" s="17">
         <v>0.5</v>
       </c>
       <c r="P23" s="14">
-        <v>0.63244</v>
+        <v>0.14881</v>
       </c>
       <c r="Q23" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="R23" s="1">
         <v>0</v>
@@ -1738,26 +1738,26 @@
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B24" s="49"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="48"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="24"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="42"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="45"/>
       <c r="O24" s="17">
         <v>1</v>
       </c>
       <c r="P24" s="14">
-        <v>0.91145799999999999</v>
+        <v>0.14881</v>
       </c>
       <c r="Q24" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="R24" s="1">
         <v>0</v>
@@ -1767,26 +1767,26 @@
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B25" s="49"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="48"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="24"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="42"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="45"/>
       <c r="O25" s="17">
         <v>2</v>
       </c>
       <c r="P25" s="14">
-        <v>3.0691999999999999</v>
+        <v>0.87425600000000003</v>
       </c>
       <c r="Q25" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="R25" s="1">
         <v>0</v>
@@ -1796,26 +1796,26 @@
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B26" s="49"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="48"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="24"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="42"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="45"/>
       <c r="O26" s="17">
         <v>4</v>
       </c>
       <c r="P26" s="14">
-        <v>7.5706800000000003</v>
+        <v>1.5439000000000001</v>
       </c>
       <c r="Q26" s="1">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="R26" s="1">
         <v>0</v>
@@ -1825,26 +1825,26 @@
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B27" s="49"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="48"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="24"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="42"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="45"/>
       <c r="O27" s="17">
         <v>8</v>
       </c>
       <c r="P27" s="14">
-        <v>14.3973</v>
+        <v>8.5751500000000007</v>
       </c>
       <c r="Q27" s="1">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="R27" s="1">
         <v>0</v>
@@ -1864,18 +1864,18 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="9"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="24">
+      <c r="M28" s="44"/>
+      <c r="N28" s="45">
         <v>16</v>
       </c>
       <c r="O28" s="17">
         <v>0.5</v>
       </c>
       <c r="P28" s="14">
-        <v>0.27901799999999999</v>
+        <v>0.14881</v>
       </c>
       <c r="Q28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R28" s="1">
         <v>0</v>
@@ -1885,25 +1885,25 @@
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="33"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="24"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="27"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="45"/>
       <c r="O29" s="17">
         <v>1</v>
       </c>
       <c r="P29" s="14">
-        <v>0.46503</v>
+        <v>0.70684499999999995</v>
       </c>
       <c r="Q29" s="1">
         <v>1</v>
@@ -1916,23 +1916,23 @@
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B30" s="34"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="33"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="24"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="27"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="45"/>
       <c r="O30" s="17">
         <v>2</v>
       </c>
       <c r="P30" s="14">
-        <v>0.42782700000000001</v>
+        <v>1.84152</v>
       </c>
       <c r="Q30" s="1">
         <v>3</v>
@@ -1945,26 +1945,26 @@
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B31" s="34"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="33"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="24"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="27"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="45"/>
       <c r="O31" s="17">
         <v>4</v>
       </c>
       <c r="P31" s="14">
-        <v>0.29761900000000002</v>
+        <v>4.1294599999999999</v>
       </c>
       <c r="Q31" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R31" s="1">
         <v>0</v>
@@ -1974,23 +1974,23 @@
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B32" s="34"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="33"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="24"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="27"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="45"/>
       <c r="O32" s="17">
         <v>8</v>
       </c>
       <c r="P32" s="14">
-        <v>0.40922599999999998</v>
+        <v>3.53423</v>
       </c>
       <c r="Q32" s="1">
         <v>3</v>
@@ -2003,30 +2003,30 @@
       </c>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B33" s="34"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="33"/>
-      <c r="M33" s="26">
+      <c r="B33" s="28"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="27"/>
+      <c r="M33" s="44">
         <v>3</v>
       </c>
-      <c r="N33" s="24">
+      <c r="N33" s="45">
         <v>1</v>
       </c>
       <c r="O33" s="17">
         <v>0.5</v>
       </c>
       <c r="P33" s="14">
-        <v>5.0781200000000002</v>
+        <v>0.87425600000000003</v>
       </c>
       <c r="Q33" s="1">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="R33" s="1">
         <v>0</v>
@@ -2036,26 +2036,26 @@
       </c>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B34" s="34"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="33"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="24"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="27"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="45"/>
       <c r="O34" s="17">
         <v>1</v>
       </c>
       <c r="P34" s="14">
-        <v>7.9055099999999996</v>
+        <v>0.76264900000000002</v>
       </c>
       <c r="Q34" s="1">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="R34" s="1">
         <v>0</v>
@@ -2065,26 +2065,26 @@
       </c>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B35" s="34"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="33"/>
-      <c r="M35" s="26"/>
-      <c r="N35" s="24"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="27"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="45"/>
       <c r="O35" s="17">
         <v>2</v>
       </c>
       <c r="P35" s="14">
-        <v>14.453099999999999</v>
+        <v>4.2224700000000004</v>
       </c>
       <c r="Q35" s="1">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="R35" s="1">
         <v>0</v>
@@ -2094,26 +2094,26 @@
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B36" s="34"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="33"/>
-      <c r="M36" s="26"/>
-      <c r="N36" s="24"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="27"/>
+      <c r="M36" s="44"/>
+      <c r="N36" s="45"/>
       <c r="O36" s="17">
         <v>4</v>
       </c>
       <c r="P36" s="14">
-        <v>24.535</v>
+        <v>13.485900000000001</v>
       </c>
       <c r="Q36" s="1">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="R36" s="1">
         <v>0</v>
@@ -2123,26 +2123,26 @@
       </c>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B37" s="34"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="33"/>
-      <c r="M37" s="26"/>
-      <c r="N37" s="24"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="27"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="45"/>
       <c r="O37" s="17">
         <v>8</v>
       </c>
       <c r="P37" s="14">
-        <v>39.267099999999999</v>
+        <v>30.3385</v>
       </c>
       <c r="Q37" s="1">
-        <v>152</v>
+        <v>67</v>
       </c>
       <c r="R37" s="1">
         <v>0</v>
@@ -2162,18 +2162,18 @@
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="9"/>
-      <c r="M38" s="26"/>
-      <c r="N38" s="24">
+      <c r="M38" s="44"/>
+      <c r="N38" s="45">
         <v>4</v>
       </c>
       <c r="O38" s="17">
         <v>0.5</v>
       </c>
       <c r="P38" s="14">
-        <v>0.44642900000000002</v>
+        <v>0.14881</v>
       </c>
       <c r="Q38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R38" s="1">
         <v>0</v>
@@ -2183,28 +2183,28 @@
       </c>
     </row>
     <row r="39" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="31"/>
-      <c r="M39" s="26"/>
-      <c r="N39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="25"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="45"/>
       <c r="O39" s="17">
         <v>1</v>
       </c>
       <c r="P39" s="14">
-        <v>0.85565500000000005</v>
+        <v>0.33482099999999998</v>
       </c>
       <c r="Q39" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R39" s="1">
         <v>0</v>
@@ -2214,23 +2214,23 @@
       </c>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B40" s="29"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="31"/>
-      <c r="M40" s="26"/>
-      <c r="N40" s="24"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="25"/>
+      <c r="M40" s="44"/>
+      <c r="N40" s="45"/>
       <c r="O40" s="17">
         <v>2</v>
       </c>
       <c r="P40" s="14">
-        <v>0.72544600000000004</v>
+        <v>0.50223200000000001</v>
       </c>
       <c r="Q40" s="1">
         <v>2</v>
@@ -2243,26 +2243,26 @@
       </c>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B41" s="29"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="31"/>
-      <c r="M41" s="26"/>
-      <c r="N41" s="24"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="25"/>
+      <c r="M41" s="44"/>
+      <c r="N41" s="45"/>
       <c r="O41" s="17">
         <v>4</v>
       </c>
       <c r="P41" s="14">
-        <v>1.07887</v>
+        <v>2.1205400000000001</v>
       </c>
       <c r="Q41" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R41" s="1">
         <v>0</v>
@@ -2272,26 +2272,26 @@
       </c>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B42" s="29"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="31"/>
-      <c r="M42" s="26"/>
-      <c r="N42" s="24"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="25"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="45"/>
       <c r="O42" s="17">
         <v>8</v>
       </c>
       <c r="P42" s="14">
-        <v>1.07887</v>
+        <v>3.8876499999999998</v>
       </c>
       <c r="Q42" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R42" s="1">
         <v>0</v>
@@ -2301,28 +2301,28 @@
       </c>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B43" s="29"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="31"/>
-      <c r="M43" s="26"/>
-      <c r="N43" s="24">
+      <c r="B43" s="23"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="25"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="45">
         <v>16</v>
       </c>
       <c r="O43" s="17">
         <v>0.5</v>
       </c>
       <c r="P43" s="14">
-        <v>0.390625</v>
+        <v>0.26041700000000001</v>
       </c>
       <c r="Q43" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R43" s="1">
         <v>0</v>
@@ -2332,26 +2332,26 @@
       </c>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B44" s="29"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="31"/>
-      <c r="M44" s="26"/>
-      <c r="N44" s="24"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="25"/>
+      <c r="M44" s="44"/>
+      <c r="N44" s="45"/>
       <c r="O44" s="17">
         <v>1</v>
       </c>
       <c r="P44" s="14">
-        <v>0.63244</v>
+        <v>1.3392900000000001</v>
       </c>
       <c r="Q44" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R44" s="1">
         <v>0</v>
@@ -2371,13 +2371,13 @@
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
       <c r="K45" s="12"/>
-      <c r="M45" s="26"/>
-      <c r="N45" s="24"/>
+      <c r="M45" s="44"/>
+      <c r="N45" s="45"/>
       <c r="O45" s="17">
         <v>2</v>
       </c>
       <c r="P45" s="14">
-        <v>0.48363099999999998</v>
+        <v>3.81324</v>
       </c>
       <c r="Q45" s="1">
         <v>2</v>
@@ -2390,28 +2390,28 @@
       </c>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="33"/>
-      <c r="M46" s="26"/>
-      <c r="N46" s="24"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="27"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="45"/>
       <c r="O46" s="17">
         <v>4</v>
       </c>
       <c r="P46" s="14">
-        <v>0.52083299999999999</v>
+        <v>6.4546099999999997</v>
       </c>
       <c r="Q46" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R46" s="1">
         <v>0</v>
@@ -2421,26 +2421,26 @@
       </c>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B47" s="34"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="33"/>
-      <c r="M47" s="26"/>
-      <c r="N47" s="24"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="27"/>
+      <c r="M47" s="44"/>
+      <c r="N47" s="45"/>
       <c r="O47" s="17">
         <v>8</v>
       </c>
       <c r="P47" s="14">
-        <v>0.35342299999999999</v>
+        <v>1.07887</v>
       </c>
       <c r="Q47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R47" s="1">
         <v>0</v>
@@ -2450,30 +2450,30 @@
       </c>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B48" s="34"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="33"/>
-      <c r="M48" s="26">
+      <c r="B48" s="28"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="27"/>
+      <c r="M48" s="44">
         <v>4</v>
       </c>
-      <c r="N48" s="24">
+      <c r="N48" s="45">
         <v>1</v>
       </c>
       <c r="O48" s="17">
         <v>0.5</v>
       </c>
       <c r="P48" s="14">
-        <v>3.4226200000000002</v>
+        <v>0.223214</v>
       </c>
       <c r="Q48" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="R48" s="1">
         <v>0</v>
@@ -2483,26 +2483,26 @@
       </c>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B49" s="34"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="33"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="24"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="27"/>
+      <c r="M49" s="44"/>
+      <c r="N49" s="45"/>
       <c r="O49" s="17">
         <v>1</v>
       </c>
       <c r="P49" s="14">
-        <v>5.2455400000000001</v>
+        <v>1.46949</v>
       </c>
       <c r="Q49" s="1">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="R49" s="1">
         <v>0</v>
@@ -2512,26 +2512,26 @@
       </c>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B50" s="34"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="33"/>
-      <c r="M50" s="26"/>
-      <c r="N50" s="24"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="27"/>
+      <c r="M50" s="44"/>
+      <c r="N50" s="45"/>
       <c r="O50" s="17">
         <v>2</v>
       </c>
       <c r="P50" s="14">
-        <v>11.5327</v>
+        <v>3.5900300000000001</v>
       </c>
       <c r="Q50" s="1">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="R50" s="1">
         <v>0</v>
@@ -2541,26 +2541,26 @@
       </c>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B51" s="34"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="33"/>
-      <c r="M51" s="26"/>
-      <c r="N51" s="24"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="27"/>
+      <c r="M51" s="44"/>
+      <c r="N51" s="45"/>
       <c r="O51" s="17">
         <v>4</v>
       </c>
       <c r="P51" s="14">
-        <v>21.0565</v>
+        <v>9.2819900000000004</v>
       </c>
       <c r="Q51" s="1">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="R51" s="1">
         <v>0</v>
@@ -2570,26 +2570,26 @@
       </c>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B52" s="34"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="33"/>
-      <c r="M52" s="26"/>
-      <c r="N52" s="24"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="27"/>
+      <c r="M52" s="44"/>
+      <c r="N52" s="45"/>
       <c r="O52" s="17">
         <v>8</v>
       </c>
       <c r="P52" s="14">
-        <v>31.9754</v>
+        <v>22.767900000000001</v>
       </c>
       <c r="Q52" s="1">
-        <v>139</v>
+        <v>45</v>
       </c>
       <c r="R52" s="1">
         <v>0</v>
@@ -2599,28 +2599,28 @@
       </c>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B53" s="34"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="32"/>
-      <c r="I53" s="32"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="33"/>
-      <c r="M53" s="26"/>
-      <c r="N53" s="24">
+      <c r="B53" s="28"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="27"/>
+      <c r="M53" s="44"/>
+      <c r="N53" s="45">
         <v>4</v>
       </c>
       <c r="O53" s="17">
         <v>0.5</v>
       </c>
       <c r="P53" s="14">
-        <v>0.55803599999999998</v>
+        <v>0</v>
       </c>
       <c r="Q53" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R53" s="1">
         <v>0</v>
@@ -2630,26 +2630,26 @@
       </c>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B54" s="34"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="33"/>
-      <c r="M54" s="26"/>
-      <c r="N54" s="24"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="27"/>
+      <c r="M54" s="44"/>
+      <c r="N54" s="45"/>
       <c r="O54" s="17">
         <v>1</v>
       </c>
       <c r="P54" s="14">
-        <v>0.539435</v>
+        <v>0</v>
       </c>
       <c r="Q54" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R54" s="1">
         <v>0</v>
@@ -2659,26 +2659,26 @@
       </c>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B55" s="34"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="33"/>
-      <c r="M55" s="26"/>
-      <c r="N55" s="24"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="27"/>
+      <c r="M55" s="44"/>
+      <c r="N55" s="45"/>
       <c r="O55" s="17">
         <v>2</v>
       </c>
       <c r="P55" s="14">
-        <v>0.61383900000000002</v>
+        <v>1.8229200000000001</v>
       </c>
       <c r="Q55" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R55" s="1">
         <v>0</v>
@@ -2688,26 +2688,26 @@
       </c>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B56" s="34"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="33"/>
-      <c r="M56" s="26"/>
-      <c r="N56" s="24"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="27"/>
+      <c r="M56" s="44"/>
+      <c r="N56" s="45"/>
       <c r="O56" s="17">
         <v>4</v>
       </c>
       <c r="P56" s="14">
-        <v>0.46503</v>
+        <v>2.1949399999999999</v>
       </c>
       <c r="Q56" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R56" s="1">
         <v>0</v>
@@ -2717,26 +2717,26 @@
       </c>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B57" s="34"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="33"/>
-      <c r="M57" s="26"/>
-      <c r="N57" s="24"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="27"/>
+      <c r="M57" s="44"/>
+      <c r="N57" s="45"/>
       <c r="O57" s="17">
         <v>8</v>
       </c>
       <c r="P57" s="14">
-        <v>0.26041700000000001</v>
+        <v>3.40402</v>
       </c>
       <c r="Q57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R57" s="1">
         <v>0</v>
@@ -2746,28 +2746,28 @@
       </c>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B58" s="34"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="32"/>
-      <c r="J58" s="32"/>
-      <c r="K58" s="33"/>
-      <c r="M58" s="26"/>
-      <c r="N58" s="24">
+      <c r="B58" s="28"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="27"/>
+      <c r="M58" s="44"/>
+      <c r="N58" s="45">
         <v>16</v>
       </c>
       <c r="O58" s="17">
         <v>0.5</v>
       </c>
       <c r="P58" s="14">
-        <v>0.33482099999999998</v>
+        <v>3.7202399999999997E-2</v>
       </c>
       <c r="Q58" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R58" s="1">
         <v>0</v>
@@ -2777,26 +2777,26 @@
       </c>
     </row>
     <row r="59" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B59" s="34"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="32"/>
-      <c r="J59" s="32"/>
-      <c r="K59" s="33"/>
-      <c r="M59" s="26"/>
-      <c r="N59" s="24"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="27"/>
+      <c r="M59" s="44"/>
+      <c r="N59" s="45"/>
       <c r="O59" s="17">
         <v>1</v>
       </c>
       <c r="P59" s="14">
-        <v>0.26041700000000001</v>
+        <v>2.4739599999999999</v>
       </c>
       <c r="Q59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R59" s="1">
         <v>0</v>
@@ -2806,26 +2806,26 @@
       </c>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B60" s="34"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
-      <c r="J60" s="32"/>
-      <c r="K60" s="33"/>
-      <c r="M60" s="26"/>
-      <c r="N60" s="24"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="27"/>
+      <c r="M60" s="44"/>
+      <c r="N60" s="45"/>
       <c r="O60" s="17">
         <v>2</v>
       </c>
       <c r="P60" s="14">
-        <v>0.14881</v>
+        <v>2.34375</v>
       </c>
       <c r="Q60" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R60" s="1">
         <v>0</v>
@@ -2835,26 +2835,26 @@
       </c>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B61" s="34"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="32"/>
-      <c r="J61" s="32"/>
-      <c r="K61" s="33"/>
-      <c r="M61" s="26"/>
-      <c r="N61" s="24"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="27"/>
+      <c r="M61" s="44"/>
+      <c r="N61" s="45"/>
       <c r="O61" s="17">
         <v>4</v>
       </c>
       <c r="P61" s="14">
-        <v>0.31622</v>
+        <v>2.7715800000000002</v>
       </c>
       <c r="Q61" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R61" s="1">
         <v>0</v>
@@ -2864,26 +2864,26 @@
       </c>
     </row>
     <row r="62" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="35"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="36"/>
-      <c r="J62" s="36"/>
-      <c r="K62" s="37"/>
-      <c r="M62" s="27"/>
-      <c r="N62" s="28"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="30"/>
+      <c r="H62" s="30"/>
+      <c r="I62" s="30"/>
+      <c r="J62" s="30"/>
+      <c r="K62" s="31"/>
+      <c r="M62" s="46"/>
+      <c r="N62" s="47"/>
       <c r="O62" s="18">
         <v>8</v>
       </c>
       <c r="P62" s="15">
-        <v>0.31622</v>
+        <v>2.6971699999999998</v>
       </c>
       <c r="Q62" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R62" s="3">
         <v>0</v>
@@ -2894,12 +2894,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B39:K44"/>
-    <mergeCell ref="B46:K62"/>
-    <mergeCell ref="B2:K4"/>
-    <mergeCell ref="B6:K9"/>
-    <mergeCell ref="B11:K27"/>
-    <mergeCell ref="B29:K37"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="N8:N12"/>
+    <mergeCell ref="N13:N17"/>
+    <mergeCell ref="M3:M17"/>
+    <mergeCell ref="M18:M32"/>
+    <mergeCell ref="N18:N22"/>
+    <mergeCell ref="N23:N27"/>
+    <mergeCell ref="N28:N32"/>
     <mergeCell ref="M33:M47"/>
     <mergeCell ref="N33:N37"/>
     <mergeCell ref="N38:N42"/>
@@ -2908,14 +2910,12 @@
     <mergeCell ref="N48:N52"/>
     <mergeCell ref="N53:N57"/>
     <mergeCell ref="N58:N62"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="N8:N12"/>
-    <mergeCell ref="N13:N17"/>
-    <mergeCell ref="M3:M17"/>
-    <mergeCell ref="M18:M32"/>
-    <mergeCell ref="N18:N22"/>
-    <mergeCell ref="N23:N27"/>
-    <mergeCell ref="N28:N32"/>
+    <mergeCell ref="B39:K44"/>
+    <mergeCell ref="B46:K62"/>
+    <mergeCell ref="B2:K4"/>
+    <mergeCell ref="B6:K9"/>
+    <mergeCell ref="B11:K27"/>
+    <mergeCell ref="B29:K37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>